<commit_message>
fix issue 105 - import pendidikanLanjutan
</commit_message>
<xml_diff>
--- a/public/template/Template Import Lowongan Pendidikan Lanjutan.xlsx
+++ b/public/template/Template Import Lowongan Pendidikan Lanjutan.xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zasieun/code/lms/public/template/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE60C40-1067-0A42-9B32-0B60A5BADB6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{2042C5AB-5029-3345-8BA1-985777DC723C}"/>
+    <workbookView windowWidth="15860" windowHeight="11840"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Referensi" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -37,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
   <si>
     <t>No</t>
   </si>
@@ -45,6 +36,9 @@
     <t>Program Studi</t>
   </si>
   <si>
+    <t>Instansi</t>
+  </si>
+  <si>
     <t>Jenjang</t>
   </si>
   <si>
@@ -60,115 +54,199 @@
     <t>Batas Usia</t>
   </si>
   <si>
+    <t>Jumlah Formasi</t>
+  </si>
+  <si>
+    <t>Tahun</t>
+  </si>
+  <si>
     <t>Catatan</t>
   </si>
   <si>
+    <t>Data</t>
+  </si>
+  <si>
     <t>Pengisian</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>Strata I</t>
   </si>
   <si>
+    <t>strata_1</t>
+  </si>
+  <si>
+    <t>Diberhentikan dari Jabatan</t>
+  </si>
+  <si>
+    <t>diberhentikan_dari_jabatan</t>
+  </si>
+  <si>
     <t>Strata II</t>
   </si>
   <si>
+    <t>strata_2</t>
+  </si>
+  <si>
+    <t>Tidak Diberhentikan dari Jabatan</t>
+  </si>
+  <si>
+    <t>tidak_diberhentikan_dari_jabatan</t>
+  </si>
+  <si>
     <t>Strata III</t>
   </si>
   <si>
+    <t>strata_3</t>
+  </si>
+  <si>
     <t>Profesi, PPDS (Dokter Spesialis)</t>
   </si>
   <si>
+    <t>profesi_ppds</t>
+  </si>
+  <si>
     <t>PPDS (Dokter Subspesialis)</t>
   </si>
   <si>
+    <t>ppds_subspesialis</t>
+  </si>
+  <si>
+    <t>APBD</t>
+  </si>
+  <si>
+    <t>apbd</t>
+  </si>
+  <si>
+    <t>Non APBD</t>
+  </si>
+  <si>
+    <t>non_apbd</t>
+  </si>
+  <si>
+    <t>Mandiri</t>
+  </si>
+  <si>
+    <t>mandiri</t>
+  </si>
+  <si>
     <t>Juru (Ia)</t>
   </si>
   <si>
+    <t>juru_ia</t>
+  </si>
+  <si>
     <t>Juru Muda Tingkat I (Ib)</t>
   </si>
   <si>
+    <t>juru_muda_tingkat_i_ib</t>
+  </si>
+  <si>
+    <t>Juru (Ic)</t>
+  </si>
+  <si>
+    <t>juru_ic</t>
+  </si>
+  <si>
     <t>Juru Tingkat I (Id)</t>
   </si>
   <si>
+    <t>juru_tingkat_i_id</t>
+  </si>
+  <si>
     <t>Pengatur (IIa)</t>
   </si>
   <si>
+    <t>pengatur_iia</t>
+  </si>
+  <si>
     <t>Pengatur Muda Tingkat I (IIb)</t>
   </si>
   <si>
+    <t>pengatur_muda_tingkat_i_iib</t>
+  </si>
+  <si>
     <t>Pengatur (IIc)</t>
   </si>
   <si>
+    <t>pengatur_iic</t>
+  </si>
+  <si>
     <t>Pengatur Tingkat I (IId)</t>
   </si>
   <si>
+    <t>pengatur_tingkat_i_iid</t>
+  </si>
+  <si>
     <t>Penata (IIIa)</t>
   </si>
   <si>
+    <t>penata_iiia</t>
+  </si>
+  <si>
     <t>Penata Muda Tingkat I (IIIb)</t>
   </si>
   <si>
+    <t>penata_muda_tingkat_i_iiib</t>
+  </si>
+  <si>
     <t>Penata (IIIc)</t>
   </si>
   <si>
+    <t>penata_iiic</t>
+  </si>
+  <si>
     <t>Penata Tingkat I (IIId)</t>
   </si>
   <si>
+    <t>penata_tingkat_i_iiid</t>
+  </si>
+  <si>
     <t>Pembina (IVa)</t>
   </si>
   <si>
+    <t>pembina_iva</t>
+  </si>
+  <si>
     <t>Pembina Tingkat I (IVb)</t>
   </si>
   <si>
+    <t>pembina_tingkat_i_ivb</t>
+  </si>
+  <si>
     <t>Pembina Utama Muda (IVc)</t>
   </si>
   <si>
+    <t>pembina_utama_muda_ivc</t>
+  </si>
+  <si>
     <t>Pembina Utama Madya (IVd)</t>
   </si>
   <si>
+    <t>pembina_utama_madya_ivd</t>
+  </si>
+  <si>
     <t>Pembina Utama (IVe)</t>
   </si>
   <si>
-    <t>Profesi</t>
-  </si>
-  <si>
-    <t>PPDS</t>
-  </si>
-  <si>
-    <t>Diberhentikan dari Jabatan</t>
-  </si>
-  <si>
-    <t>Tidak Diberhentikan dari Jabatan</t>
-  </si>
-  <si>
-    <t>APBD</t>
-  </si>
-  <si>
-    <t>Non APBD</t>
-  </si>
-  <si>
-    <t>Mandiri</t>
-  </si>
-  <si>
-    <t>Tahun</t>
-  </si>
-  <si>
-    <t>Jumlah Formasi</t>
+    <t>pembina_utama_ive</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -176,10 +254,162 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,12 +418,192 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -203,39 +613,325 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -284,7 +980,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -317,26 +1013,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -369,23 +1048,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -547,37 +1209,32 @@
       </a:style>
     </a:lnDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2DBD29-0B10-1A4A-84B4-30C29AEAB459}">
-  <dimension ref="A1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B2" sqref="B2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6"/>
   <cols>
-    <col min="1" max="1" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.5" customWidth="1"/>
+    <col min="2" max="2" width="12.8303571428571" customWidth="1"/>
+    <col min="3" max="4" width="7.33035714285714" customWidth="1"/>
+    <col min="5" max="5" width="16.6607142857143" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="10.1607142857143" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="14.1607142857143" customWidth="1"/>
+    <col min="10" max="11" width="7.83035714285714" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,16 +1257,19 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -622,8 +1282,9 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -636,8 +1297,9 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -650,8 +1312,9 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -664,8 +1327,9 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -678,8 +1342,9 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -692,8 +1357,9 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -706,8 +1372,9 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -720,8 +1387,9 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -734,348 +1402,365 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC0456F3-105F-3D4E-99E9-97BB671A0E2B}">
-  <dimension ref="B3:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B3:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="17.6" outlineLevelCol="7"/>
   <cols>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.8839285714286" customWidth="1"/>
+    <col min="4" max="4" width="30.2053571428571" customWidth="1"/>
+    <col min="7" max="7" width="34.2232142857143" customWidth="1"/>
+    <col min="8" max="8" width="38.8392857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8">
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
       <c r="B4" s="2">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5" s="2">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
       <c r="B6" s="2">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
       <c r="B7" s="2">
         <v>4</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
       <c r="B8" s="2">
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="6:8">
       <c r="F9" s="2">
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="6:8">
       <c r="F10" s="2">
         <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
       <c r="B12" s="2">
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
       <c r="B13" s="2">
         <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4">
       <c r="B14" s="2">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
       <c r="B15" s="2">
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
       <c r="B16" s="2">
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
       <c r="B17" s="2">
         <v>6</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4">
       <c r="B18" s="2">
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4">
       <c r="B19" s="2">
         <v>8</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4">
       <c r="B20" s="2">
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4">
       <c r="B21" s="2">
         <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4">
       <c r="B22" s="2">
         <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4">
       <c r="B23" s="2">
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4">
       <c r="B24" s="2">
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4">
       <c r="B25" s="2">
         <v>14</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4">
       <c r="B26" s="2">
         <v>15</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4">
       <c r="B27" s="2">
         <v>16</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>30</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4">
+      <c r="B28" s="2">
+        <v>17</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix import pendidikan lanjutan
</commit_message>
<xml_diff>
--- a/public/template/Template Import Lowongan Pendidikan Lanjutan.xlsx
+++ b/public/template/Template Import Lowongan Pendidikan Lanjutan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zasieun/code/lms/public/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zasieun/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8EA03C-3E19-1049-8901-BB5C3C8F4F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCEB6D8-7312-734F-9A45-4F18895D87FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="54">
   <si>
     <t>No</t>
   </si>
@@ -172,6 +172,30 @@
   </si>
   <si>
     <t>Universitas</t>
+  </si>
+  <si>
+    <t>Syarat Pendidikan</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SMP</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>D-1</t>
+  </si>
+  <si>
+    <t>D-2</t>
+  </si>
+  <si>
+    <t>D-3</t>
+  </si>
+  <si>
+    <t>D-4</t>
   </si>
 </sst>
 </file>
@@ -208,7 +232,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,12 +279,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +600,7 @@
     <col min="11" max="12" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,43 +634,48 @@
       <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L2" s="3"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L3" s="3"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -654,8 +690,9 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -670,8 +707,9 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -686,8 +724,9 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -702,8 +741,9 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -718,8 +758,9 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -734,8 +775,9 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -750,6 +792,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -762,7 +805,7 @@
   <dimension ref="B3:H28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:H10"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,6 +970,15 @@
       <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
@@ -938,6 +990,15 @@
       <c r="D13" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
@@ -949,6 +1010,15 @@
       <c r="D14" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
@@ -960,6 +1030,15 @@
       <c r="D15" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F15" s="2">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
@@ -971,8 +1050,17 @@
       <c r="D16" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F16" s="2">
+        <v>4</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>6</v>
       </c>
@@ -982,8 +1070,17 @@
       <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F17" s="2">
+        <v>5</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>7</v>
       </c>
@@ -993,8 +1090,17 @@
       <c r="D18" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F18" s="2">
+        <v>6</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>8</v>
       </c>
@@ -1004,8 +1110,17 @@
       <c r="D19" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="2">
+        <v>7</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>9</v>
       </c>
@@ -1015,8 +1130,17 @@
       <c r="D20" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F20" s="2">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>10</v>
       </c>
@@ -1026,8 +1150,17 @@
       <c r="D21" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F21" s="2">
+        <v>9</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>11</v>
       </c>
@@ -1037,8 +1170,17 @@
       <c r="D22" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F22" s="2">
+        <v>10</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>12</v>
       </c>
@@ -1049,7 +1191,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>13</v>
       </c>
@@ -1060,7 +1202,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>14</v>
       </c>
@@ -1071,7 +1213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>15</v>
       </c>
@@ -1082,7 +1224,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>16</v>
       </c>
@@ -1093,7 +1235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>17</v>
       </c>

</xml_diff>